<commit_message>
upload the holding register
</commit_message>
<xml_diff>
--- a/document/MODBUS_ADDR_DEFINITION.xlsx
+++ b/document/MODBUS_ADDR_DEFINITION.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\career\custum_enviorument\arduino-nightly-windows\Modbus_slave\ProjectModbus\document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E27878B-FA90-4DE5-99AD-13E835FE8F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ADDRESS</t>
   </si>
@@ -34,18 +28,6 @@
   </si>
   <si>
     <t>holding register</t>
-  </si>
-  <si>
-    <t>Serial configuration</t>
-  </si>
-  <si>
-    <t>Serial baudrate</t>
-  </si>
-  <si>
-    <t>network timeout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device Id </t>
   </si>
   <si>
     <t>VARIABLE DETIAL</t>
@@ -73,24 +55,6 @@
     <t xml:space="preserve">input register </t>
   </si>
   <si>
-    <t>count 1b</t>
-  </si>
-  <si>
-    <t>count 1a</t>
-  </si>
-  <si>
-    <t>count 1c</t>
-  </si>
-  <si>
-    <t>count 2a</t>
-  </si>
-  <si>
-    <t>count 2b</t>
-  </si>
-  <si>
-    <t>count 2c</t>
-  </si>
-  <si>
     <t>store shift A count</t>
   </si>
   <si>
@@ -103,22 +67,134 @@
     <t xml:space="preserve">last count epoch time </t>
   </si>
   <si>
-    <t>count_1 last event (MSB)</t>
-  </si>
-  <si>
-    <t>count_1 last event (LSB)</t>
-  </si>
-  <si>
-    <t>count_2 last event (MSB)</t>
-  </si>
-  <si>
-    <t>count_2 last event (LSB)</t>
+    <t>debouncing time for input button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no event occur in this time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">command to get holding register </t>
+  </si>
+  <si>
+    <t>Device Id (int)</t>
+  </si>
+  <si>
+    <t>Serial configuration(int16_t)</t>
+  </si>
+  <si>
+    <t>Serial baudrate(int16_t)</t>
+  </si>
+  <si>
+    <t>network timeout(int16_t)</t>
+  </si>
+  <si>
+    <t>debouncing time(int16_t)</t>
+  </si>
+  <si>
+    <t>count 1a(uint16_t)</t>
+  </si>
+  <si>
+    <t>count 1b(uint16_t)</t>
+  </si>
+  <si>
+    <t>count 1c(uint16_t)</t>
+  </si>
+  <si>
+    <t>count 2a(uint16_t)</t>
+  </si>
+  <si>
+    <t>count 2b(uint16_t)</t>
+  </si>
+  <si>
+    <t>count 2c(uint16_t)</t>
+  </si>
+  <si>
+    <r>
+      <t>count_1 last event (MSB)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[16bit]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>count_1 last event (LSB)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[16bit]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>count_2 last event (LSB)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[16bit]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>count_2 last event (MSB)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[16bit]</t>
+    </r>
+  </si>
+  <si>
+    <t>RTC current time (LSB)[int16_t]</t>
+  </si>
+  <si>
+    <t>RTC current time (MSB)[int16_t]</t>
+  </si>
+  <si>
+    <t>update value by writing '1' on address 40007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">command to get rtc value </t>
+  </si>
+  <si>
+    <t>0x01,0x03,0x00,0x00,0x00,0x0A,0xC5,0xCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x01,0x06,0x00,0x06,0x00,0x01,0xA8,0x0B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,47 +414,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -387,25 +432,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -414,35 +440,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +596,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -539,7 +631,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -716,18 +808,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,223 +836,295 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40001</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" spans="2:7" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15"/>
+      <c r="C3" s="3">
+        <v>40002</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="2:7" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="14">
+        <v>40003</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
+      <c r="C5" s="14">
+        <v>40004</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="2:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
+      <c r="C6" s="34">
+        <v>40005</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="36"/>
+    </row>
+    <row r="7" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
+      <c r="C7" s="14">
+        <v>40006</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="2:7" s="38" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="37"/>
+      <c r="C8" s="38">
+        <v>40007</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="36"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9">
-        <v>40001</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C9" s="16">
+        <v>30011</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="2:7" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="36"/>
-      <c r="C3" s="10">
-        <v>40002</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="13">
+        <v>30012</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="2:7" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="35">
-        <v>40003</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="13">
+        <v>30013</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9">
-        <v>40004</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="13">
+        <v>30014</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="37">
-        <v>30011</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="25"/>
-      <c r="C7" s="34">
-        <v>30012</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="25"/>
-      <c r="C8" s="34">
-        <v>30013</v>
-      </c>
-      <c r="D8" s="28" t="s">
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="13">
+        <v>30015</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="16">
+        <v>30021</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="13">
+        <v>30022</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="13">
+        <v>30023</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="13">
+        <v>30024</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="C18" s="17">
+        <v>30025</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
-      <c r="C9" s="34">
-        <v>30014</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="25"/>
-      <c r="C10" s="34">
-        <v>30015</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
-      <c r="C11" s="37">
-        <v>30021</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
-      <c r="C12" s="34">
-        <v>30022</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
-      <c r="C13" s="34">
-        <v>30023</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
-      <c r="C14" s="34">
-        <v>30024</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="26"/>
-      <c r="C15" s="38">
-        <v>30025</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="29"/>
+    </row>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E15:G15"/>
+  <mergeCells count="22">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>